<commit_message>
update the models worksheets
</commit_message>
<xml_diff>
--- a/assets/worksheets/template-cliente.xlsx
+++ b/assets/worksheets/template-cliente.xlsx
@@ -355,7 +355,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="41">
+  <borders count="40">
     <border/>
     <border>
       <left style="thin">
@@ -526,15 +526,15 @@
     </border>
     <border>
       <left/>
-      <right/>
       <top/>
     </border>
     <border>
+      <top/>
+    </border>
+    <border>
       <left/>
-      <top/>
-    </border>
-    <border>
-      <left/>
+    </border>
+    <border>
       <right/>
     </border>
     <border>
@@ -595,9 +595,6 @@
       <top/>
     </border>
     <border>
-      <top/>
-    </border>
-    <border>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -629,20 +626,6 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -651,7 +634,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="94">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -724,42 +707,38 @@
     <xf borderId="24" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="24" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="25" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="25" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="26" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
+    <xf borderId="27" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="9" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="27" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
     <xf borderId="28" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
+    <xf borderId="29" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
     <xf borderId="16" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="29" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="29" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="30" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="30" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="30" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="31" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="31" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="32" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="32" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="33" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="34" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="25" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="34" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="35" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="24" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="35" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="36" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="9" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
@@ -788,9 +767,6 @@
     <xf borderId="4" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="6" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf borderId="9" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -830,17 +806,11 @@
     </xf>
     <xf borderId="38" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="39" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="15" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="27" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf borderId="40" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="9" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="38" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
@@ -854,7 +824,7 @@
     <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="29" fillId="0" fontId="1" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="30" fillId="0" fontId="1" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="9" fillId="0" fontId="1" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -866,10 +836,10 @@
     <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="29" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="30" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="29" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="30" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -911,7 +881,7 @@
     <xdr:ext cx="2381250" cy="0"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr descr="LOGO.jpg" id="0" name="image3.jpg"/>
+        <xdr:cNvPr descr="LOGO.jpg" id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -939,7 +909,7 @@
     <xdr:ext cx="542925" cy="133350"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Imagem"/>
+        <xdr:cNvPr id="0" name="image5.png" title="Imagem"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -967,7 +937,7 @@
     <xdr:ext cx="571500" cy="104775"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Imagem"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Imagem"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -995,7 +965,7 @@
     <xdr:ext cx="2200275" cy="304800"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.png" title="Imagem"/>
+        <xdr:cNvPr id="0" name="image4.png" title="Imagem"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1023,7 +993,7 @@
     <xdr:ext cx="914400" cy="304800"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image4.png" title="Imagem"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Imagem"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1051,7 +1021,7 @@
     <xdr:ext cx="914400" cy="304800"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image4.png" title="Imagem"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Imagem"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1400,144 +1370,143 @@
         <v>9</v>
       </c>
       <c r="E9" s="34"/>
-      <c r="F9" s="35"/>
+      <c r="F9" s="32"/>
       <c r="G9" s="31" t="s">
         <v>10</v>
       </c>
       <c r="H9" s="32"/>
-      <c r="I9" s="36" t="s">
+      <c r="I9" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="J9" s="37"/>
-      <c r="K9" s="37"/>
+      <c r="K9" s="36"/>
       <c r="L9" s="6"/>
     </row>
     <row r="10" ht="18.0" customHeight="1">
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="37" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="20"/>
-      <c r="D10" s="39" t="s">
+      <c r="D10" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="40" t="s">
+      <c r="E10" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="38" t="s">
+      <c r="F10" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="39" t="s">
+      <c r="G10" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="41" t="s">
+      <c r="H10" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="42"/>
-      <c r="J10" s="43"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="42"/>
       <c r="K10" s="13"/>
-      <c r="L10" s="44"/>
+      <c r="L10" s="43"/>
     </row>
     <row r="11" ht="16.5" customHeight="1">
-      <c r="B11" s="45" t="s">
+      <c r="B11" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="46" t="s">
+      <c r="C11" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="47"/>
-      <c r="H11" s="47"/>
-      <c r="I11" s="47"/>
-      <c r="J11" s="47"/>
-      <c r="K11" s="48"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="47"/>
       <c r="L11" s="6"/>
     </row>
     <row r="12" ht="16.5" customHeight="1">
-      <c r="B12" s="49" t="s">
+      <c r="B12" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="50" t="s">
+      <c r="C12" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="51"/>
-      <c r="E12" s="51"/>
-      <c r="F12" s="51"/>
-      <c r="G12" s="51"/>
-      <c r="H12" s="51"/>
-      <c r="I12" s="51"/>
-      <c r="J12" s="51"/>
-      <c r="K12" s="52"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="50"/>
       <c r="L12" s="6"/>
     </row>
     <row r="13" ht="12.0" customHeight="1">
-      <c r="B13" s="53" t="s">
+      <c r="B13" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="43"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="43"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="42"/>
       <c r="K13" s="13"/>
       <c r="L13" s="6"/>
     </row>
     <row r="14" ht="25.5" customHeight="1">
-      <c r="B14" s="54" t="s">
+      <c r="B14" s="52" t="s">
         <v>21</v>
       </c>
       <c r="C14" s="8"/>
-      <c r="D14" s="54" t="s">
+      <c r="D14" s="52" t="s">
         <v>22</v>
       </c>
       <c r="E14" s="8"/>
-      <c r="F14" s="55" t="s">
+      <c r="F14" s="53" t="s">
         <v>23</v>
       </c>
       <c r="H14" s="8"/>
-      <c r="I14" s="55" t="s">
+      <c r="I14" s="53" t="s">
         <v>24</v>
       </c>
       <c r="J14" s="8"/>
-      <c r="K14" s="56" t="s">
+      <c r="K14" s="54" t="s">
         <v>25</v>
       </c>
       <c r="L14" s="6"/>
     </row>
     <row r="15" ht="21.0" customHeight="1">
-      <c r="B15" s="57" t="s">
+      <c r="B15" s="55" t="s">
         <v>26</v>
       </c>
       <c r="C15" s="13"/>
-      <c r="D15" s="58" t="s">
+      <c r="D15" s="56" t="s">
         <v>27</v>
       </c>
       <c r="E15" s="13"/>
-      <c r="F15" s="59" t="s">
+      <c r="F15" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="43"/>
-      <c r="H15" s="43"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
       <c r="I15" s="13"/>
-      <c r="J15" s="57" t="s">
+      <c r="J15" s="55" t="s">
         <v>29</v>
       </c>
       <c r="K15" s="13"/>
       <c r="L15" s="6"/>
     </row>
     <row r="16" ht="13.5" customHeight="1">
-      <c r="B16" s="60" t="s">
+      <c r="B16" s="58" t="s">
         <v>30</v>
       </c>
       <c r="K16" s="8"/>
       <c r="L16" s="6"/>
     </row>
     <row r="17" ht="18.75" customHeight="1">
-      <c r="B17" s="61"/>
+      <c r="B17" s="59"/>
       <c r="K17" s="8"/>
       <c r="L17" s="6"/>
     </row>
@@ -1552,35 +1521,27 @@
       <c r="L19" s="6"/>
     </row>
     <row r="20" ht="18.75" customHeight="1">
-      <c r="B20" s="62"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="10"/>
+      <c r="B20" s="7"/>
+      <c r="K20" s="8"/>
       <c r="L20" s="6"/>
     </row>
     <row r="21" ht="18.0" customHeight="1">
-      <c r="B21" s="63" t="s">
+      <c r="B21" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="43"/>
-      <c r="I21" s="43"/>
-      <c r="J21" s="43"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="42"/>
       <c r="K21" s="13"/>
       <c r="L21" s="6"/>
     </row>
     <row r="22" ht="18.75" customHeight="1">
-      <c r="B22" s="61"/>
+      <c r="B22" s="59"/>
       <c r="K22" s="8"/>
       <c r="L22" s="6"/>
     </row>
@@ -1595,20 +1556,12 @@
       <c r="L24" s="6"/>
     </row>
     <row r="25" ht="18.75" customHeight="1">
-      <c r="B25" s="62"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="10"/>
+      <c r="B25" s="7"/>
+      <c r="K25" s="8"/>
       <c r="L25" s="6"/>
     </row>
     <row r="26" ht="13.5" customHeight="1">
-      <c r="B26" s="64" t="s">
+      <c r="B26" s="61" t="s">
         <v>32</v>
       </c>
       <c r="C26" s="11"/>
@@ -1623,7 +1576,7 @@
       <c r="L26" s="6"/>
     </row>
     <row r="27" ht="18.75" customHeight="1">
-      <c r="B27" s="61"/>
+      <c r="B27" s="59"/>
       <c r="K27" s="8"/>
       <c r="L27" s="6"/>
     </row>
@@ -1638,66 +1591,58 @@
       <c r="L29" s="6"/>
     </row>
     <row r="30" ht="18.0" customHeight="1">
-      <c r="B30" s="62"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="10"/>
+      <c r="B30" s="7"/>
+      <c r="K30" s="8"/>
       <c r="L30" s="6"/>
     </row>
     <row r="31" ht="18.75" customHeight="1">
-      <c r="B31" s="65" t="s">
+      <c r="B31" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="43"/>
-      <c r="D31" s="43"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="66" t="s">
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="H31" s="43"/>
-      <c r="I31" s="43"/>
-      <c r="J31" s="43"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="42"/>
+      <c r="J31" s="42"/>
       <c r="K31" s="13"/>
       <c r="L31" s="6"/>
     </row>
     <row r="32" ht="18.75" customHeight="1">
-      <c r="B32" s="67"/>
-      <c r="C32" s="43"/>
-      <c r="D32" s="43"/>
-      <c r="E32" s="43"/>
-      <c r="F32" s="43"/>
-      <c r="G32" s="68"/>
-      <c r="H32" s="43"/>
-      <c r="I32" s="43"/>
-      <c r="J32" s="43"/>
+      <c r="B32" s="64"/>
+      <c r="C32" s="42"/>
+      <c r="D32" s="42"/>
+      <c r="E32" s="42"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="65"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="42"/>
+      <c r="J32" s="42"/>
       <c r="K32" s="13"/>
       <c r="L32" s="6"/>
     </row>
     <row r="33" ht="18.75" customHeight="1">
-      <c r="B33" s="69"/>
-      <c r="C33" s="43"/>
-      <c r="D33" s="43"/>
-      <c r="E33" s="43"/>
-      <c r="F33" s="43"/>
-      <c r="G33" s="43"/>
-      <c r="H33" s="43"/>
-      <c r="I33" s="43"/>
-      <c r="J33" s="43"/>
+      <c r="B33" s="66"/>
+      <c r="C33" s="42"/>
+      <c r="D33" s="42"/>
+      <c r="E33" s="42"/>
+      <c r="F33" s="42"/>
+      <c r="G33" s="42"/>
+      <c r="H33" s="42"/>
+      <c r="I33" s="42"/>
+      <c r="J33" s="42"/>
       <c r="K33" s="13"/>
       <c r="L33" s="6"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="B34" s="70" t="s">
+      <c r="B34" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="71" t="s">
+      <c r="C34" s="68" t="s">
         <v>36</v>
       </c>
       <c r="D34" s="11"/>
@@ -1711,7 +1656,7 @@
       <c r="L34" s="6"/>
     </row>
     <row r="35" ht="13.5" customHeight="1">
-      <c r="B35" s="72" t="s">
+      <c r="B35" s="69" t="s">
         <v>37</v>
       </c>
       <c r="C35" s="11"/>
@@ -1726,7 +1671,7 @@
       <c r="L35" s="6"/>
     </row>
     <row r="36" ht="18.75" customHeight="1">
-      <c r="B36" s="61"/>
+      <c r="B36" s="59"/>
       <c r="K36" s="8"/>
       <c r="L36" s="6"/>
     </row>
@@ -1741,133 +1686,125 @@
       <c r="L38" s="6"/>
     </row>
     <row r="39" ht="18.75" customHeight="1">
-      <c r="B39" s="62"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="11"/>
-      <c r="J39" s="11"/>
-      <c r="K39" s="10"/>
+      <c r="B39" s="7"/>
+      <c r="K39" s="8"/>
       <c r="L39" s="6"/>
     </row>
     <row r="40" ht="15.0" customHeight="1">
-      <c r="B40" s="73" t="s">
+      <c r="B40" s="70" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="74" t="s">
+      <c r="C40" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="D40" s="43"/>
+      <c r="D40" s="42"/>
       <c r="E40" s="13"/>
-      <c r="F40" s="75" t="s">
+      <c r="F40" s="72" t="s">
         <v>40</v>
       </c>
       <c r="G40" s="3"/>
-      <c r="H40" s="74" t="s">
+      <c r="H40" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="I40" s="43"/>
-      <c r="J40" s="43"/>
+      <c r="I40" s="42"/>
+      <c r="J40" s="42"/>
       <c r="K40" s="13"/>
       <c r="L40" s="6"/>
     </row>
     <row r="41" ht="15.0" customHeight="1">
-      <c r="B41" s="76"/>
-      <c r="C41" s="74" t="s">
+      <c r="B41" s="73"/>
+      <c r="C41" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="D41" s="43"/>
+      <c r="D41" s="42"/>
       <c r="E41" s="13"/>
       <c r="F41" s="7"/>
       <c r="G41" s="8"/>
-      <c r="H41" s="74" t="s">
+      <c r="H41" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="I41" s="43"/>
-      <c r="J41" s="43"/>
+      <c r="I41" s="42"/>
+      <c r="J41" s="42"/>
       <c r="K41" s="13"/>
       <c r="L41" s="6"/>
     </row>
     <row r="42" ht="15.0" customHeight="1">
-      <c r="B42" s="77"/>
-      <c r="C42" s="74" t="s">
+      <c r="B42" s="74"/>
+      <c r="C42" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="D42" s="43"/>
+      <c r="D42" s="42"/>
       <c r="E42" s="13"/>
       <c r="F42" s="9"/>
       <c r="G42" s="10"/>
-      <c r="H42" s="74" t="s">
+      <c r="H42" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
+      <c r="I42" s="42"/>
+      <c r="J42" s="42"/>
       <c r="K42" s="13"/>
       <c r="L42" s="6"/>
     </row>
     <row r="43" ht="18.0" customHeight="1">
-      <c r="B43" s="78" t="s">
+      <c r="B43" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="C43" s="79"/>
-      <c r="D43" s="78" t="s">
+      <c r="C43" s="20"/>
+      <c r="D43" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="E43" s="79"/>
-      <c r="F43" s="80" t="s">
+      <c r="E43" s="20"/>
+      <c r="F43" s="76" t="s">
         <v>44</v>
       </c>
-      <c r="G43" s="81"/>
-      <c r="H43" s="20"/>
-      <c r="I43" s="80" t="s">
+      <c r="G43" s="42"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="J43" s="79"/>
-      <c r="K43" s="21"/>
+      <c r="J43" s="42"/>
+      <c r="K43" s="13"/>
       <c r="L43" s="6"/>
     </row>
     <row r="44">
-      <c r="B44" s="82" t="s">
+      <c r="B44" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="C44" s="83" t="s">
+      <c r="C44" s="78" t="s">
         <v>47</v>
       </c>
       <c r="D44" s="8"/>
-      <c r="E44" s="83" t="s">
+      <c r="E44" s="78" t="s">
         <v>48</v>
       </c>
       <c r="F44" s="8"/>
-      <c r="G44" s="84" t="s">
+      <c r="G44" s="79" t="s">
         <v>49</v>
       </c>
       <c r="H44" s="11"/>
       <c r="I44" s="10"/>
-      <c r="J44" s="84" t="s">
+      <c r="J44" s="79" t="s">
         <v>50</v>
       </c>
       <c r="K44" s="10"/>
       <c r="L44" s="6"/>
     </row>
     <row r="45">
-      <c r="B45" s="76"/>
-      <c r="C45" s="85" t="s">
+      <c r="B45" s="73"/>
+      <c r="C45" s="80" t="s">
         <v>51</v>
       </c>
       <c r="D45" s="13"/>
-      <c r="E45" s="86">
+      <c r="E45" s="81">
         <v>0.0</v>
       </c>
       <c r="F45" s="13"/>
-      <c r="G45" s="87">
+      <c r="G45" s="82">
         <v>0.0</v>
       </c>
-      <c r="H45" s="43"/>
+      <c r="H45" s="42"/>
       <c r="I45" s="13"/>
-      <c r="J45" s="88">
+      <c r="J45" s="83">
         <f>G45-E45</f>
         <v>0</v>
       </c>
@@ -1875,37 +1812,37 @@
       <c r="L45" s="6"/>
     </row>
     <row r="46">
-      <c r="B46" s="76"/>
-      <c r="C46" s="89"/>
+      <c r="B46" s="73"/>
+      <c r="C46" s="84"/>
       <c r="D46" s="13"/>
-      <c r="E46" s="90"/>
+      <c r="E46" s="85"/>
       <c r="F46" s="13"/>
-      <c r="G46" s="89"/>
-      <c r="H46" s="43"/>
+      <c r="G46" s="84"/>
+      <c r="H46" s="42"/>
       <c r="I46" s="13"/>
-      <c r="J46" s="91"/>
-      <c r="K46" s="91"/>
+      <c r="J46" s="86"/>
+      <c r="K46" s="86"/>
       <c r="L46" s="6"/>
     </row>
     <row r="47">
-      <c r="B47" s="77"/>
-      <c r="C47" s="92"/>
+      <c r="B47" s="74"/>
+      <c r="C47" s="87"/>
       <c r="D47" s="13"/>
-      <c r="E47" s="90"/>
+      <c r="E47" s="85"/>
       <c r="F47" s="13"/>
-      <c r="G47" s="89"/>
-      <c r="H47" s="43"/>
+      <c r="G47" s="84"/>
+      <c r="H47" s="42"/>
       <c r="I47" s="13"/>
-      <c r="J47" s="91"/>
-      <c r="K47" s="91"/>
+      <c r="J47" s="86"/>
+      <c r="K47" s="86"/>
       <c r="L47" s="6"/>
     </row>
     <row r="48" ht="18.75" customHeight="1">
-      <c r="B48" s="93" t="s">
+      <c r="B48" s="88" t="s">
         <v>52</v>
       </c>
       <c r="F48" s="8"/>
-      <c r="G48" s="94" t="s">
+      <c r="G48" s="89" t="s">
         <v>52</v>
       </c>
       <c r="K48" s="8"/>
@@ -1924,18 +1861,18 @@
       <c r="L50" s="6"/>
     </row>
     <row r="51" ht="21.0" customHeight="1">
-      <c r="B51" s="95" t="s">
+      <c r="B51" s="90" t="s">
         <v>53</v>
       </c>
       <c r="F51" s="8"/>
-      <c r="G51" s="96" t="s">
+      <c r="G51" s="91" t="s">
         <v>54</v>
       </c>
       <c r="K51" s="8"/>
       <c r="L51" s="6"/>
     </row>
     <row r="52" ht="18.75" customHeight="1">
-      <c r="B52" s="97" t="s">
+      <c r="B52" s="92" t="s">
         <v>55</v>
       </c>
       <c r="C52" s="2"/>
@@ -1950,7 +1887,7 @@
       <c r="L52" s="6"/>
     </row>
     <row r="53" ht="19.5" customHeight="1">
-      <c r="B53" s="98" t="s">
+      <c r="B53" s="93" t="s">
         <v>56</v>
       </c>
       <c r="C53" s="11"/>
@@ -2913,28 +2850,27 @@
     <row r="1000"/>
     <row r="1001"/>
   </sheetData>
-  <mergeCells count="76">
-    <mergeCell ref="B22:K24"/>
-    <mergeCell ref="B25:K25"/>
+  <mergeCells count="77">
     <mergeCell ref="B26:K26"/>
-    <mergeCell ref="B27:K29"/>
-    <mergeCell ref="B30:K30"/>
     <mergeCell ref="B31:F31"/>
     <mergeCell ref="G31:K31"/>
+    <mergeCell ref="B22:K25"/>
+    <mergeCell ref="B27:K30"/>
     <mergeCell ref="B32:F32"/>
     <mergeCell ref="G32:K32"/>
     <mergeCell ref="B33:K33"/>
     <mergeCell ref="C34:K34"/>
     <mergeCell ref="B35:K35"/>
-    <mergeCell ref="B36:K38"/>
-    <mergeCell ref="B39:K39"/>
+    <mergeCell ref="B36:K39"/>
     <mergeCell ref="E45:F45"/>
     <mergeCell ref="C46:D46"/>
     <mergeCell ref="E46:F46"/>
     <mergeCell ref="C47:D47"/>
     <mergeCell ref="E47:F47"/>
+    <mergeCell ref="B48:F50"/>
     <mergeCell ref="B51:F51"/>
-    <mergeCell ref="B48:F50"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
     <mergeCell ref="B40:B42"/>
     <mergeCell ref="C40:E40"/>
     <mergeCell ref="F40:G42"/>
@@ -2942,6 +2878,15 @@
     <mergeCell ref="C42:E42"/>
     <mergeCell ref="B44:B47"/>
     <mergeCell ref="E44:F44"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="B7:C8"/>
+    <mergeCell ref="D7:G8"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="D9:F9"/>
     <mergeCell ref="B2:D5"/>
     <mergeCell ref="E2:I5"/>
     <mergeCell ref="J2:K4"/>
@@ -2953,13 +2898,6 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B7:C8"/>
-    <mergeCell ref="D7:G8"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="G9:H9"/>
     <mergeCell ref="I10:K10"/>
     <mergeCell ref="C11:K11"/>
     <mergeCell ref="C12:K12"/>
@@ -2971,25 +2909,25 @@
     <mergeCell ref="F15:I15"/>
     <mergeCell ref="J15:K15"/>
     <mergeCell ref="B16:K16"/>
-    <mergeCell ref="B20:K20"/>
     <mergeCell ref="B21:K21"/>
-    <mergeCell ref="B17:K19"/>
+    <mergeCell ref="B17:K20"/>
     <mergeCell ref="C44:D44"/>
     <mergeCell ref="C45:D45"/>
     <mergeCell ref="G45:I45"/>
     <mergeCell ref="G46:I46"/>
     <mergeCell ref="G47:I47"/>
+    <mergeCell ref="G48:K50"/>
     <mergeCell ref="G51:K51"/>
     <mergeCell ref="B52:K52"/>
     <mergeCell ref="B53:K53"/>
-    <mergeCell ref="G48:K50"/>
     <mergeCell ref="H40:K40"/>
     <mergeCell ref="H41:K41"/>
     <mergeCell ref="H42:K42"/>
-    <mergeCell ref="G43:H43"/>
     <mergeCell ref="G44:I44"/>
     <mergeCell ref="J44:K44"/>
     <mergeCell ref="J45:K45"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="I43:K43"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.28" footer="0.0" header="0.0" left="0.17" right="0.2" top="0.15748031496062992"/>

</xml_diff>

<commit_message>
Made the dynamic creation of the basic info. part of the client form
</commit_message>
<xml_diff>
--- a/assets/worksheets/template-cliente.xlsx
+++ b/assets/worksheets/template-cliente.xlsx
@@ -482,6 +482,14 @@
       </bottom>
     </border>
     <border>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
       <right/>
       <top style="thin">
         <color rgb="FF000000"/>
@@ -552,14 +560,6 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -666,25 +666,23 @@
     </xf>
     <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="13" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="14" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="15" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="16" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="17" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="16" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf borderId="18" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="18" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="19" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf borderId="19" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="20" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="top"/>
@@ -692,40 +690,42 @@
     <xf borderId="1" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="20" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="21" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="22" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="6" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="top"/>
     </xf>
     <xf borderId="6" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="22" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="23" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="23" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="24" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="24" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="25" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="25" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="26" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="26" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="23" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="27" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="27" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="28" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="9" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="28" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
     <xf borderId="29" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
+    <xf borderId="30" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
     <xf borderId="16" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="30" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="30" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="17" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
@@ -736,7 +736,7 @@
     <xf borderId="33" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="34" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="35" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="24" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="25" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="36" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -744,10 +744,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -824,7 +824,7 @@
     <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="30" fillId="0" fontId="1" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="17" fillId="0" fontId="1" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="9" fillId="0" fontId="1" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -836,10 +836,10 @@
     <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="30" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="17" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="30" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="17" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -881,7 +881,7 @@
     <xdr:ext cx="2381250" cy="0"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr descr="LOGO.jpg" id="0" name="image2.jpg"/>
+        <xdr:cNvPr descr="LOGO.jpg" id="0" name="image4.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -909,7 +909,7 @@
     <xdr:ext cx="542925" cy="133350"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.png" title="Imagem"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Imagem"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -965,7 +965,7 @@
     <xdr:ext cx="2200275" cy="304800"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image4.png" title="Imagem"/>
+        <xdr:cNvPr id="0" name="image5.png" title="Imagem"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1371,38 +1371,38 @@
       </c>
       <c r="E9" s="34"/>
       <c r="F9" s="32"/>
-      <c r="G9" s="31" t="s">
+      <c r="G9" s="35" t="s">
         <v>10</v>
       </c>
       <c r="H9" s="32"/>
-      <c r="I9" s="35" t="s">
+      <c r="I9" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="K9" s="36"/>
+      <c r="K9" s="37"/>
       <c r="L9" s="6"/>
     </row>
     <row r="10" ht="18.0" customHeight="1">
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="38" t="s">
+      <c r="C10" s="21"/>
+      <c r="D10" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="39" t="s">
+      <c r="E10" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="37" t="s">
+      <c r="F10" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="38" t="s">
+      <c r="G10" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="40" t="s">
+      <c r="H10" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="41"/>
-      <c r="J10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="20"/>
       <c r="K10" s="13"/>
       <c r="L10" s="43"/>
     </row>
@@ -1444,14 +1444,14 @@
       <c r="B13" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="42"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
       <c r="K13" s="13"/>
       <c r="L13" s="6"/>
     </row>
@@ -1460,15 +1460,15 @@
         <v>21</v>
       </c>
       <c r="C14" s="8"/>
-      <c r="D14" s="52" t="s">
+      <c r="D14" s="53" t="s">
         <v>22</v>
       </c>
       <c r="E14" s="8"/>
-      <c r="F14" s="53" t="s">
+      <c r="F14" s="52" t="s">
         <v>23</v>
       </c>
       <c r="H14" s="8"/>
-      <c r="I14" s="53" t="s">
+      <c r="I14" s="52" t="s">
         <v>24</v>
       </c>
       <c r="J14" s="8"/>
@@ -1489,8 +1489,8 @@
       <c r="F15" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
       <c r="I15" s="13"/>
       <c r="J15" s="55" t="s">
         <v>29</v>
@@ -1529,14 +1529,14 @@
       <c r="B21" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="42"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="42"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
       <c r="K21" s="13"/>
       <c r="L21" s="6"/>
     </row>
@@ -1599,42 +1599,42 @@
       <c r="B31" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="42"/>
-      <c r="D31" s="42"/>
-      <c r="E31" s="42"/>
-      <c r="F31" s="42"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
       <c r="G31" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="H31" s="42"/>
-      <c r="I31" s="42"/>
-      <c r="J31" s="42"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
       <c r="K31" s="13"/>
       <c r="L31" s="6"/>
     </row>
     <row r="32" ht="18.75" customHeight="1">
       <c r="B32" s="64"/>
-      <c r="C32" s="42"/>
-      <c r="D32" s="42"/>
-      <c r="E32" s="42"/>
-      <c r="F32" s="42"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
       <c r="G32" s="65"/>
-      <c r="H32" s="42"/>
-      <c r="I32" s="42"/>
-      <c r="J32" s="42"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20"/>
       <c r="K32" s="13"/>
       <c r="L32" s="6"/>
     </row>
     <row r="33" ht="18.75" customHeight="1">
       <c r="B33" s="66"/>
-      <c r="C33" s="42"/>
-      <c r="D33" s="42"/>
-      <c r="E33" s="42"/>
-      <c r="F33" s="42"/>
-      <c r="G33" s="42"/>
-      <c r="H33" s="42"/>
-      <c r="I33" s="42"/>
-      <c r="J33" s="42"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="20"/>
       <c r="K33" s="13"/>
       <c r="L33" s="6"/>
     </row>
@@ -1697,7 +1697,7 @@
       <c r="C40" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="D40" s="42"/>
+      <c r="D40" s="20"/>
       <c r="E40" s="13"/>
       <c r="F40" s="72" t="s">
         <v>40</v>
@@ -1706,8 +1706,8 @@
       <c r="H40" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="I40" s="42"/>
-      <c r="J40" s="42"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="20"/>
       <c r="K40" s="13"/>
       <c r="L40" s="6"/>
     </row>
@@ -1716,15 +1716,15 @@
       <c r="C41" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="D41" s="42"/>
+      <c r="D41" s="20"/>
       <c r="E41" s="13"/>
       <c r="F41" s="7"/>
       <c r="G41" s="8"/>
       <c r="H41" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="I41" s="42"/>
-      <c r="J41" s="42"/>
+      <c r="I41" s="20"/>
+      <c r="J41" s="20"/>
       <c r="K41" s="13"/>
       <c r="L41" s="6"/>
     </row>
@@ -1733,15 +1733,15 @@
       <c r="C42" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="D42" s="42"/>
+      <c r="D42" s="20"/>
       <c r="E42" s="13"/>
       <c r="F42" s="9"/>
       <c r="G42" s="10"/>
       <c r="H42" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="I42" s="42"/>
-      <c r="J42" s="42"/>
+      <c r="I42" s="20"/>
+      <c r="J42" s="20"/>
       <c r="K42" s="13"/>
       <c r="L42" s="6"/>
     </row>
@@ -1749,20 +1749,20 @@
       <c r="B43" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="C43" s="20"/>
+      <c r="C43" s="21"/>
       <c r="D43" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="E43" s="20"/>
+      <c r="E43" s="21"/>
       <c r="F43" s="76" t="s">
         <v>44</v>
       </c>
-      <c r="G43" s="42"/>
+      <c r="G43" s="20"/>
       <c r="H43" s="13"/>
       <c r="I43" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="J43" s="42"/>
+      <c r="J43" s="20"/>
       <c r="K43" s="13"/>
       <c r="L43" s="6"/>
     </row>
@@ -1802,7 +1802,7 @@
       <c r="G45" s="82">
         <v>0.0</v>
       </c>
-      <c r="H45" s="42"/>
+      <c r="H45" s="20"/>
       <c r="I45" s="13"/>
       <c r="J45" s="83">
         <f>G45-E45</f>
@@ -1818,7 +1818,7 @@
       <c r="E46" s="85"/>
       <c r="F46" s="13"/>
       <c r="G46" s="84"/>
-      <c r="H46" s="42"/>
+      <c r="H46" s="20"/>
       <c r="I46" s="13"/>
       <c r="J46" s="86"/>
       <c r="K46" s="86"/>
@@ -1831,7 +1831,7 @@
       <c r="E47" s="85"/>
       <c r="F47" s="13"/>
       <c r="G47" s="84"/>
-      <c r="H47" s="42"/>
+      <c r="H47" s="20"/>
       <c r="I47" s="13"/>
       <c r="J47" s="86"/>
       <c r="K47" s="86"/>
@@ -2851,83 +2851,83 @@
     <row r="1001"/>
   </sheetData>
   <mergeCells count="77">
-    <mergeCell ref="B26:K26"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="G31:K31"/>
-    <mergeCell ref="B22:K25"/>
-    <mergeCell ref="B27:K30"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="G32:K32"/>
-    <mergeCell ref="B33:K33"/>
-    <mergeCell ref="C34:K34"/>
-    <mergeCell ref="B35:K35"/>
+    <mergeCell ref="H41:K41"/>
+    <mergeCell ref="H42:K42"/>
     <mergeCell ref="B36:K39"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="B48:F50"/>
-    <mergeCell ref="B51:F51"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
     <mergeCell ref="B40:B42"/>
     <mergeCell ref="C40:E40"/>
     <mergeCell ref="F40:G42"/>
+    <mergeCell ref="H40:K40"/>
     <mergeCell ref="C41:E41"/>
     <mergeCell ref="C42:E42"/>
+    <mergeCell ref="G44:I44"/>
+    <mergeCell ref="J44:K44"/>
+    <mergeCell ref="G45:I45"/>
+    <mergeCell ref="J45:K45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="B48:F50"/>
+    <mergeCell ref="B51:F51"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="G47:I47"/>
+    <mergeCell ref="G48:K50"/>
+    <mergeCell ref="G51:K51"/>
+    <mergeCell ref="B52:K52"/>
+    <mergeCell ref="B53:K53"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="I43:K43"/>
     <mergeCell ref="B44:B47"/>
     <mergeCell ref="E44:F44"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="G46:I46"/>
+    <mergeCell ref="B2:D5"/>
+    <mergeCell ref="E2:I5"/>
+    <mergeCell ref="J2:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="I6:K6"/>
     <mergeCell ref="B7:C8"/>
     <mergeCell ref="D7:G8"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="J7:K7"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="J8:K8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="I9:K9"/>
     <mergeCell ref="D9:F9"/>
-    <mergeCell ref="B2:D5"/>
-    <mergeCell ref="E2:I5"/>
-    <mergeCell ref="J2:K4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="G9:H9"/>
     <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
     <mergeCell ref="I10:K10"/>
     <mergeCell ref="C11:K11"/>
     <mergeCell ref="C12:K12"/>
     <mergeCell ref="B13:K13"/>
+    <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="F14:H14"/>
     <mergeCell ref="I14:J14"/>
+    <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:E15"/>
+    <mergeCell ref="J15:K15"/>
     <mergeCell ref="F15:I15"/>
-    <mergeCell ref="J15:K15"/>
     <mergeCell ref="B16:K16"/>
+    <mergeCell ref="B17:K20"/>
     <mergeCell ref="B21:K21"/>
-    <mergeCell ref="B17:K20"/>
-    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="B22:K25"/>
+    <mergeCell ref="B26:K26"/>
+    <mergeCell ref="B27:K30"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="G31:K31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="G32:K32"/>
+    <mergeCell ref="B33:K33"/>
+    <mergeCell ref="C34:K34"/>
+    <mergeCell ref="B35:K35"/>
     <mergeCell ref="C45:D45"/>
-    <mergeCell ref="G45:I45"/>
-    <mergeCell ref="G46:I46"/>
-    <mergeCell ref="G47:I47"/>
-    <mergeCell ref="G48:K50"/>
-    <mergeCell ref="G51:K51"/>
-    <mergeCell ref="B52:K52"/>
-    <mergeCell ref="B53:K53"/>
-    <mergeCell ref="H40:K40"/>
-    <mergeCell ref="H41:K41"/>
-    <mergeCell ref="H42:K42"/>
-    <mergeCell ref="G44:I44"/>
-    <mergeCell ref="J44:K44"/>
-    <mergeCell ref="J45:K45"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="I43:K43"/>
+    <mergeCell ref="E45:F45"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.28" footer="0.0" header="0.0" left="0.17" right="0.2" top="0.15748031496062992"/>

</xml_diff>

<commit_message>
Made the dynamic creation of the services  part of the client form
</commit_message>
<xml_diff>
--- a/assets/worksheets/template-cliente.xlsx
+++ b/assets/worksheets/template-cliente.xlsx
@@ -11,7 +11,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="70">
+  <si>
+    <t xml:space="preserve">             </t>
+  </si>
   <si>
     <t>RELATÓRIO DE ATENDIMENTO</t>
   </si>
@@ -19,24 +22,36 @@
     <t xml:space="preserve">XXXXXX </t>
   </si>
   <si>
+    <t xml:space="preserve">     </t>
+  </si>
+  <si>
     <t xml:space="preserve">DATA: </t>
   </si>
   <si>
     <t>Cliente:</t>
   </si>
   <si>
+    <t xml:space="preserve">       </t>
+  </si>
+  <si>
     <t>O.S:</t>
   </si>
   <si>
     <t>Local de Atendimento:</t>
   </si>
   <si>
+    <t xml:space="preserve">      </t>
+  </si>
+  <si>
     <t xml:space="preserve">    [    ]     CORRETIVA</t>
   </si>
   <si>
     <t xml:space="preserve"> [    ]     PREVENTIVA</t>
   </si>
   <si>
+    <t xml:space="preserve">                           </t>
+  </si>
+  <si>
     <t>Solicitado por:</t>
   </si>
   <si>
@@ -46,9 +61,6 @@
     <t>Atendido por:</t>
   </si>
   <si>
-    <t>Atendente</t>
-  </si>
-  <si>
     <t xml:space="preserve">Máquina Parada:          </t>
   </si>
   <si>
@@ -59,6 +71,9 @@
   </si>
   <si>
     <t xml:space="preserve">Garantia:          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                           </t>
   </si>
   <si>
     <t>Equipamento:</t>
@@ -166,6 +181,9 @@
     <t>DEFEITO:</t>
   </si>
   <si>
+    <t xml:space="preserve">                                        </t>
+  </si>
+  <si>
     <t>CAUSA:</t>
   </si>
   <si>
@@ -175,9 +193,15 @@
     <t>OLÉO DE MOTOR UTILIZADO</t>
   </si>
   <si>
+    <t xml:space="preserve">               </t>
+  </si>
+  <si>
     <t>OLÉO HIDRÁULICO UTILIZADO</t>
   </si>
   <si>
+    <t xml:space="preserve">                            </t>
+  </si>
+  <si>
     <t>SITUAÇÃO:</t>
   </si>
   <si>
@@ -227,6 +251,21 @@
   </si>
   <si>
     <t>00/00/0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                  </t>
   </si>
   <si>
     <t>_________________________________________</t>
@@ -286,6 +325,11 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -300,11 +344,6 @@
       <sz val="8.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -355,20 +394,99 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="57">
     <border/>
     <border>
-      <left style="thin">
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+    </border>
+    <border>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
         <color rgb="FF000000"/>
       </left>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-    </border>
-    <border>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
       <right style="thin">
@@ -377,16 +495,93 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <bottom/>
+    </border>
+    <border>
+      <right/>
+      <bottom/>
+    </border>
+    <border>
+      <left/>
+      <bottom/>
+    </border>
+    <border>
+      <bottom/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <left/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
     </border>
     <border>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <right/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
       <left style="thin">
@@ -397,20 +592,33 @@
       </bottom>
     </border>
     <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <top/>
+    </border>
+    <border>
+      <right/>
+      <top/>
+    </border>
+    <border>
+      <left/>
+      <top/>
+    </border>
+    <border>
+      <top/>
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <top/>
+    </border>
+    <border>
+      <left/>
+    </border>
+    <border>
+      <left style="medium">
         <color rgb="FF000000"/>
       </left>
       <top style="thin">
@@ -421,129 +629,13 @@
       </bottom>
     </border>
     <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-    </border>
-    <border>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-    </border>
-    <border>
-      <left/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-    </border>
-    <border>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <left/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <right/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <top/>
-    </border>
-    <border>
-      <right/>
-      <top/>
-    </border>
-    <border>
-      <left/>
-      <top/>
-    </border>
-    <border>
-      <top/>
-    </border>
-    <border>
-      <left/>
-    </border>
-    <border>
-      <right/>
     </border>
     <border>
       <left/>
@@ -571,24 +663,56 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
       <right/>
       <bottom/>
     </border>
     <border>
-      <left/>
-      <bottom/>
-    </border>
-    <border>
-      <bottom/>
-    </border>
-    <border>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <bottom/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color rgb="FF000000"/>
       </left>
       <right/>
@@ -604,6 +728,60 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -612,7 +790,7 @@
       </top>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color rgb="FF000000"/>
       </left>
       <right style="thin">
@@ -620,7 +798,7 @@
       </right>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color rgb="FF000000"/>
       </left>
       <right style="thin">
@@ -634,12 +812,12 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="108">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -649,216 +827,240 @@
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
     <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="13" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="top"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="14" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="15" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="13" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="14" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="15" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="16" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="17" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="18" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="19" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="16" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="20" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="21" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="22" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="17" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="18" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="23" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="24" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="25" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="26" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="27" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="27" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf borderId="28" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="20" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="29" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="29" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="30" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="31" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="32" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="33" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="34" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="35" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="36" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="37" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="38" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="39" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="40" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="41" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="42" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="42" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="43" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="44" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="17" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="45" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="46" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="32" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="47" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="36" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="48" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="48" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="36" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="40" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="40" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="19" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="20" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="40" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf borderId="21" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="22" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="6" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf borderId="23" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="24" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="25" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="5" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="36" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="36" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="49" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="50" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="51" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="42" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="52" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="36" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="42" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="53" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="36" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="26" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="23" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="27" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="28" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="29" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="30" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="16" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="17" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="31" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="32" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="33" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="34" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="35" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="25" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="36" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf borderId="4" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="6" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="9" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="9" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="9" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="9" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="9" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="8" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="6" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="21" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="54" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="40" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf borderId="27" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="55" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="48" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="56" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="29" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="36" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf borderId="40" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf borderId="40" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="55" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="48" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="29" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="40" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="42" fillId="0" fontId="1" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="40" fillId="0" fontId="1" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="40" fillId="0" fontId="1" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="37" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="9" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="38" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="39" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf borderId="9" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="38" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="42" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="17" fillId="0" fontId="1" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="17" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="17" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="42" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="40" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="22" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -909,7 +1111,7 @@
     <xdr:ext cx="542925" cy="133350"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Imagem"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Imagem"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -937,7 +1139,7 @@
     <xdr:ext cx="571500" cy="104775"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Imagem"/>
+        <xdr:cNvPr id="0" name="image5.png" title="Imagem"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -965,7 +1167,7 @@
     <xdr:ext cx="2200275" cy="304800"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.png" title="Imagem"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Imagem"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -987,13 +1189,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>228600</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="914400" cy="304800"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Imagem"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Imagem"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1015,13 +1217,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>228600</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="914400" cy="304800"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Imagem"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Imagem"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1263,646 +1465,844 @@
   <sheetData>
     <row r="1" ht="5.25" customHeight="1"/>
     <row r="2">
-      <c r="B2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="C2" s="2"/>
       <c r="D2" s="3"/>
       <c r="E2" s="4" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="3"/>
       <c r="J2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="6"/>
+        <v>2</v>
+      </c>
+      <c r="K2" s="6"/>
+      <c r="L2" s="7" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" ht="15.0" customHeight="1">
-      <c r="B3" s="7"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="7"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="6"/>
+      <c r="B3" s="8"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="8"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="7" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" ht="15.0" customHeight="1">
-      <c r="B4" s="7"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="7"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="6"/>
+      <c r="B4" s="8"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="8"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="7" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="5">
-      <c r="B5" s="9"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="K5" s="13"/>
-      <c r="L5" s="6"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5" s="17"/>
+      <c r="L5" s="7" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" ht="19.5" customHeight="1">
-      <c r="B6" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="I6" s="19"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="6"/>
+      <c r="B6" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="19"/>
+      <c r="D6" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="24"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="7" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" ht="12.0" customHeight="1">
-      <c r="B7" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="K7" s="3"/>
-      <c r="L7" s="6"/>
+      <c r="B7" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="26"/>
+      <c r="D7" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="29"/>
+      <c r="J7" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="29"/>
+      <c r="L7" s="7" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="B8" s="9"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="6"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="12"/>
+      <c r="J8" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="12"/>
+      <c r="L8" s="7" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="B9" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="33" t="s">
+      <c r="B9" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="37"/>
+      <c r="D9" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="39"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="37"/>
+      <c r="I9" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="34"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" s="32"/>
-      <c r="I9" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="K9" s="37"/>
-      <c r="L9" s="6"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="7" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="10" ht="18.0" customHeight="1">
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="43"/>
+      <c r="D10" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="49"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" ht="16.5" customHeight="1">
+      <c r="B11" s="51" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="52" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="53"/>
+      <c r="L11" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" ht="16.5" customHeight="1">
+      <c r="B12" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="55" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="56"/>
+      <c r="L12" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" ht="12.0" customHeight="1">
+      <c r="B13" s="57" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" ht="25.5" customHeight="1">
+      <c r="B14" s="58" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="10"/>
+      <c r="D14" s="59" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="10"/>
+      <c r="I14" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="J14" s="10"/>
+      <c r="K14" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" ht="21.0" customHeight="1">
+      <c r="B15" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="50"/>
+      <c r="D15" s="63" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="50"/>
+      <c r="F15" s="64" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" s="49"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="50"/>
+      <c r="J15" s="65" t="s">
+        <v>34</v>
+      </c>
+      <c r="K15" s="50"/>
+      <c r="L15" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" ht="15.75" customHeight="1">
+      <c r="B16" s="66" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" ht="18.75" customHeight="1">
+      <c r="B17" s="67" t="s">
+        <v>36</v>
+      </c>
+      <c r="K17" s="10"/>
+      <c r="L17" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" ht="18.75" customHeight="1">
+      <c r="B18" s="8"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" ht="18.75" customHeight="1">
+      <c r="B19" s="8"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" ht="18.75" customHeight="1">
+      <c r="B20" s="8"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" ht="16.5" customHeight="1">
+      <c r="B21" s="68" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="49"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="49"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="49"/>
+      <c r="K21" s="50"/>
+      <c r="L21" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" ht="18.75" customHeight="1">
+      <c r="B22" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="39" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="39" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" s="42"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="43"/>
-    </row>
-    <row r="11" ht="16.5" customHeight="1">
-      <c r="B11" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="45" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="46"/>
-      <c r="J11" s="46"/>
-      <c r="K11" s="47"/>
-      <c r="L11" s="6"/>
-    </row>
-    <row r="12" ht="16.5" customHeight="1">
-      <c r="B12" s="48" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="50"/>
-      <c r="L12" s="6"/>
-    </row>
-    <row r="13" ht="12.0" customHeight="1">
-      <c r="B13" s="51" t="s">
+      <c r="K22" s="10"/>
+      <c r="L22" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" ht="18.75" customHeight="1">
+      <c r="B23" s="8"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" ht="18.75" customHeight="1">
+      <c r="B24" s="8"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" ht="18.75" customHeight="1">
+      <c r="B25" s="8"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" ht="13.5" customHeight="1">
+      <c r="B26" s="68" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="49"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="49"/>
+      <c r="K26" s="50"/>
+      <c r="L26" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" ht="18.75" customHeight="1">
+      <c r="B27" s="67" t="s">
+        <v>36</v>
+      </c>
+      <c r="K27" s="10"/>
+      <c r="L27" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" ht="18.75" customHeight="1">
+      <c r="B28" s="8"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" ht="18.75" customHeight="1">
+      <c r="B29" s="8"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" ht="18.0" customHeight="1">
+      <c r="B30" s="8"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" ht="18.75" customHeight="1">
+      <c r="B31" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="6"/>
-    </row>
-    <row r="14" ht="25.5" customHeight="1">
-      <c r="B14" s="52" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="53" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="H14" s="8"/>
-      <c r="I14" s="52" t="s">
-        <v>24</v>
-      </c>
-      <c r="J14" s="8"/>
-      <c r="K14" s="54" t="s">
-        <v>25</v>
-      </c>
-      <c r="L14" s="6"/>
-    </row>
-    <row r="15" ht="21.0" customHeight="1">
-      <c r="B15" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="13"/>
-      <c r="F15" s="57" t="s">
-        <v>28</v>
-      </c>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="K15" s="13"/>
-      <c r="L15" s="6"/>
-    </row>
-    <row r="16" ht="13.5" customHeight="1">
-      <c r="B16" s="58" t="s">
-        <v>30</v>
-      </c>
-      <c r="K16" s="8"/>
-      <c r="L16" s="6"/>
-    </row>
-    <row r="17" ht="18.75" customHeight="1">
-      <c r="B17" s="59"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="6"/>
-    </row>
-    <row r="18" ht="18.75" customHeight="1">
-      <c r="B18" s="7"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="6"/>
-    </row>
-    <row r="19" ht="18.75" customHeight="1">
-      <c r="B19" s="7"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="6"/>
-    </row>
-    <row r="20" ht="18.75" customHeight="1">
-      <c r="B20" s="7"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="6"/>
-    </row>
-    <row r="21" ht="18.0" customHeight="1">
-      <c r="B21" s="60" t="s">
+      <c r="C31" s="49"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="70" t="s">
+        <v>39</v>
+      </c>
+      <c r="F31" s="71"/>
+      <c r="G31" s="72"/>
+      <c r="H31" s="73" t="s">
+        <v>40</v>
+      </c>
+      <c r="I31" s="70" t="s">
+        <v>41</v>
+      </c>
+      <c r="J31" s="71"/>
+      <c r="K31" s="74"/>
+      <c r="L31" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" ht="18.75" customHeight="1">
+      <c r="B32" s="69" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="49"/>
+      <c r="D32" s="49"/>
+      <c r="E32" s="75" t="s">
+        <v>42</v>
+      </c>
+      <c r="F32" s="2"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="73" t="s">
+        <v>40</v>
+      </c>
+      <c r="I32" s="75" t="s">
+        <v>12</v>
+      </c>
+      <c r="J32" s="2"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" ht="18.75" customHeight="1">
+      <c r="B33" s="69" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="49"/>
+      <c r="D33" s="49"/>
+      <c r="E33" s="8"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="73" t="s">
+        <v>40</v>
+      </c>
+      <c r="I33" s="8"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" ht="18.75" customHeight="1">
+      <c r="B34" s="76" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="49"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="77" t="s">
+        <v>40</v>
+      </c>
+      <c r="I34" s="13"/>
+      <c r="J34" s="14"/>
+      <c r="K34" s="78"/>
+      <c r="L34" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" ht="18.75" customHeight="1">
+      <c r="B35" s="79" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" s="49"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="49"/>
+      <c r="F35" s="49"/>
+      <c r="G35" s="49"/>
+      <c r="H35" s="49"/>
+      <c r="I35" s="49"/>
+      <c r="J35" s="49"/>
+      <c r="K35" s="50"/>
+      <c r="L35" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" ht="15.75" customHeight="1">
+      <c r="B36" s="80" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" s="81" t="s">
+        <v>44</v>
+      </c>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="24"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" ht="18.0" customHeight="1">
+      <c r="B37" s="66" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" s="24"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="24"/>
+      <c r="G37" s="24"/>
+      <c r="H37" s="24"/>
+      <c r="I37" s="24"/>
+      <c r="J37" s="24"/>
+      <c r="K37" s="12"/>
+      <c r="L37" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" ht="18.75" customHeight="1">
+      <c r="B38" s="67" t="s">
+        <v>20</v>
+      </c>
+      <c r="K38" s="10"/>
+      <c r="L38" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" ht="18.75" customHeight="1">
+      <c r="B39" s="8"/>
+      <c r="K39" s="10"/>
+      <c r="L39" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" ht="18.75" customHeight="1">
+      <c r="B40" s="8"/>
+      <c r="K40" s="10"/>
+      <c r="L40" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" ht="18.75" customHeight="1">
+      <c r="B41" s="8"/>
+      <c r="K41" s="10"/>
+      <c r="L41" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" ht="15.0" customHeight="1">
+      <c r="B42" s="82" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" s="83" t="s">
+        <v>47</v>
+      </c>
+      <c r="D42" s="49"/>
+      <c r="E42" s="50"/>
+      <c r="F42" s="84" t="s">
+        <v>48</v>
+      </c>
+      <c r="G42" s="29"/>
+      <c r="H42" s="83" t="s">
+        <v>47</v>
+      </c>
+      <c r="I42" s="49"/>
+      <c r="J42" s="49"/>
+      <c r="K42" s="50"/>
+      <c r="L42" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" ht="15.0" customHeight="1">
+      <c r="B43" s="85"/>
+      <c r="C43" s="83" t="s">
+        <v>49</v>
+      </c>
+      <c r="D43" s="49"/>
+      <c r="E43" s="50"/>
+      <c r="F43" s="86"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="83" t="s">
+        <v>49</v>
+      </c>
+      <c r="I43" s="49"/>
+      <c r="J43" s="49"/>
+      <c r="K43" s="50"/>
+      <c r="L43" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" ht="15.0" customHeight="1">
+      <c r="B44" s="87"/>
+      <c r="C44" s="83" t="s">
+        <v>50</v>
+      </c>
+      <c r="D44" s="49"/>
+      <c r="E44" s="50"/>
+      <c r="F44" s="88"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="83" t="s">
+        <v>50</v>
+      </c>
+      <c r="I44" s="49"/>
+      <c r="J44" s="49"/>
+      <c r="K44" s="50"/>
+      <c r="L44" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" ht="18.0" customHeight="1">
+      <c r="B45" s="89" t="s">
+        <v>51</v>
+      </c>
+      <c r="C45" s="43"/>
+      <c r="D45" s="90" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="6"/>
-    </row>
-    <row r="22" ht="18.75" customHeight="1">
-      <c r="B22" s="59"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="6"/>
-    </row>
-    <row r="23" ht="18.75" customHeight="1">
-      <c r="B23" s="7"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="6"/>
-    </row>
-    <row r="24" ht="18.75" customHeight="1">
-      <c r="B24" s="7"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="6"/>
-    </row>
-    <row r="25" ht="18.75" customHeight="1">
-      <c r="B25" s="7"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="6"/>
-    </row>
-    <row r="26" ht="13.5" customHeight="1">
-      <c r="B26" s="61" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="6"/>
-    </row>
-    <row r="27" ht="18.75" customHeight="1">
-      <c r="B27" s="59"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="6"/>
-    </row>
-    <row r="28" ht="18.75" customHeight="1">
-      <c r="B28" s="7"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="6"/>
-    </row>
-    <row r="29" ht="18.75" customHeight="1">
-      <c r="B29" s="7"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="6"/>
-    </row>
-    <row r="30" ht="18.0" customHeight="1">
-      <c r="B30" s="7"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="6"/>
-    </row>
-    <row r="31" ht="18.75" customHeight="1">
-      <c r="B31" s="62" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="63" t="s">
-        <v>34</v>
-      </c>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
-      <c r="K31" s="13"/>
-      <c r="L31" s="6"/>
-    </row>
-    <row r="32" ht="18.75" customHeight="1">
-      <c r="B32" s="64"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="65"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="20"/>
-      <c r="J32" s="20"/>
-      <c r="K32" s="13"/>
-      <c r="L32" s="6"/>
-    </row>
-    <row r="33" ht="18.75" customHeight="1">
-      <c r="B33" s="66"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="20"/>
-      <c r="J33" s="20"/>
-      <c r="K33" s="13"/>
-      <c r="L33" s="6"/>
-    </row>
-    <row r="34" ht="15.75" customHeight="1">
-      <c r="B34" s="67" t="s">
-        <v>35</v>
-      </c>
-      <c r="C34" s="68" t="s">
-        <v>36</v>
-      </c>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="10"/>
-      <c r="L34" s="6"/>
-    </row>
-    <row r="35" ht="13.5" customHeight="1">
-      <c r="B35" s="69" t="s">
-        <v>37</v>
-      </c>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="11"/>
-      <c r="K35" s="10"/>
-      <c r="L35" s="6"/>
-    </row>
-    <row r="36" ht="18.75" customHeight="1">
-      <c r="B36" s="59"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="6"/>
-    </row>
-    <row r="37" ht="18.75" customHeight="1">
-      <c r="B37" s="7"/>
-      <c r="K37" s="8"/>
-      <c r="L37" s="6"/>
-    </row>
-    <row r="38" ht="18.75" customHeight="1">
-      <c r="B38" s="7"/>
-      <c r="K38" s="8"/>
-      <c r="L38" s="6"/>
-    </row>
-    <row r="39" ht="18.75" customHeight="1">
-      <c r="B39" s="7"/>
-      <c r="K39" s="8"/>
-      <c r="L39" s="6"/>
-    </row>
-    <row r="40" ht="15.0" customHeight="1">
-      <c r="B40" s="70" t="s">
-        <v>38</v>
-      </c>
-      <c r="C40" s="71" t="s">
-        <v>39</v>
-      </c>
-      <c r="D40" s="20"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="72" t="s">
-        <v>40</v>
-      </c>
-      <c r="G40" s="3"/>
-      <c r="H40" s="71" t="s">
-        <v>39</v>
-      </c>
-      <c r="I40" s="20"/>
-      <c r="J40" s="20"/>
-      <c r="K40" s="13"/>
-      <c r="L40" s="6"/>
-    </row>
-    <row r="41" ht="15.0" customHeight="1">
-      <c r="B41" s="73"/>
-      <c r="C41" s="71" t="s">
-        <v>41</v>
-      </c>
-      <c r="D41" s="20"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="71" t="s">
-        <v>41</v>
-      </c>
-      <c r="I41" s="20"/>
-      <c r="J41" s="20"/>
-      <c r="K41" s="13"/>
-      <c r="L41" s="6"/>
-    </row>
-    <row r="42" ht="15.0" customHeight="1">
-      <c r="B42" s="74"/>
-      <c r="C42" s="71" t="s">
+      <c r="E45" s="43"/>
+      <c r="F45" s="91" t="s">
+        <v>52</v>
+      </c>
+      <c r="G45" s="49"/>
+      <c r="H45" s="50"/>
+      <c r="I45" s="91" t="s">
+        <v>53</v>
+      </c>
+      <c r="J45" s="49"/>
+      <c r="K45" s="50"/>
+      <c r="L45" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="B46" s="92" t="s">
+        <v>54</v>
+      </c>
+      <c r="C46" s="93" t="s">
+        <v>55</v>
+      </c>
+      <c r="D46" s="10"/>
+      <c r="E46" s="93" t="s">
+        <v>56</v>
+      </c>
+      <c r="F46" s="10"/>
+      <c r="G46" s="94" t="s">
+        <v>57</v>
+      </c>
+      <c r="H46" s="24"/>
+      <c r="I46" s="12"/>
+      <c r="J46" s="94" t="s">
+        <v>58</v>
+      </c>
+      <c r="K46" s="12"/>
+      <c r="L46" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="B47" s="85"/>
+      <c r="C47" s="95" t="s">
+        <v>59</v>
+      </c>
+      <c r="D47" s="50"/>
+      <c r="E47" s="96">
+        <v>0.0</v>
+      </c>
+      <c r="F47" s="50"/>
+      <c r="G47" s="97">
+        <v>0.0</v>
+      </c>
+      <c r="H47" s="49"/>
+      <c r="I47" s="50"/>
+      <c r="J47" s="98">
+        <f>G47-E47</f>
+        <v>0</v>
+      </c>
+      <c r="K47" s="50"/>
+      <c r="L47" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="B48" s="85"/>
+      <c r="C48" s="95" t="s">
+        <v>60</v>
+      </c>
+      <c r="D48" s="50"/>
+      <c r="E48" s="99" t="s">
+        <v>61</v>
+      </c>
+      <c r="F48" s="50"/>
+      <c r="G48" s="95" t="s">
+        <v>62</v>
+      </c>
+      <c r="H48" s="49"/>
+      <c r="I48" s="50"/>
+      <c r="J48" s="100" t="s">
+        <v>63</v>
+      </c>
+      <c r="K48" s="50"/>
+      <c r="L48" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="B49" s="87"/>
+      <c r="C49" s="101" t="s">
         <v>42</v>
       </c>
-      <c r="D42" s="20"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="71" t="s">
+      <c r="D49" s="50"/>
+      <c r="E49" s="99" t="s">
         <v>42</v>
       </c>
-      <c r="I42" s="20"/>
-      <c r="J42" s="20"/>
-      <c r="K42" s="13"/>
-      <c r="L42" s="6"/>
-    </row>
-    <row r="43" ht="18.0" customHeight="1">
-      <c r="B43" s="75" t="s">
-        <v>43</v>
-      </c>
-      <c r="C43" s="21"/>
-      <c r="D43" s="75" t="s">
-        <v>26</v>
-      </c>
-      <c r="E43" s="21"/>
-      <c r="F43" s="76" t="s">
-        <v>44</v>
-      </c>
-      <c r="G43" s="20"/>
-      <c r="H43" s="13"/>
-      <c r="I43" s="76" t="s">
-        <v>45</v>
-      </c>
-      <c r="J43" s="20"/>
-      <c r="K43" s="13"/>
-      <c r="L43" s="6"/>
-    </row>
-    <row r="44">
-      <c r="B44" s="77" t="s">
-        <v>46</v>
-      </c>
-      <c r="C44" s="78" t="s">
-        <v>47</v>
-      </c>
-      <c r="D44" s="8"/>
-      <c r="E44" s="78" t="s">
-        <v>48</v>
-      </c>
-      <c r="F44" s="8"/>
-      <c r="G44" s="79" t="s">
-        <v>49</v>
-      </c>
-      <c r="H44" s="11"/>
-      <c r="I44" s="10"/>
-      <c r="J44" s="79" t="s">
-        <v>50</v>
-      </c>
-      <c r="K44" s="10"/>
-      <c r="L44" s="6"/>
-    </row>
-    <row r="45">
-      <c r="B45" s="73"/>
-      <c r="C45" s="80" t="s">
-        <v>51</v>
-      </c>
-      <c r="D45" s="13"/>
-      <c r="E45" s="81">
-        <v>0.0</v>
-      </c>
-      <c r="F45" s="13"/>
-      <c r="G45" s="82">
-        <v>0.0</v>
-      </c>
-      <c r="H45" s="20"/>
-      <c r="I45" s="13"/>
-      <c r="J45" s="83">
-        <f>G45-E45</f>
-        <v>0</v>
-      </c>
-      <c r="K45" s="13"/>
-      <c r="L45" s="6"/>
-    </row>
-    <row r="46">
-      <c r="B46" s="73"/>
-      <c r="C46" s="84"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="85"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="84"/>
-      <c r="H46" s="20"/>
-      <c r="I46" s="13"/>
-      <c r="J46" s="86"/>
-      <c r="K46" s="86"/>
-      <c r="L46" s="6"/>
-    </row>
-    <row r="47">
-      <c r="B47" s="74"/>
-      <c r="C47" s="87"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="85"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="84"/>
-      <c r="H47" s="20"/>
-      <c r="I47" s="13"/>
-      <c r="J47" s="86"/>
-      <c r="K47" s="86"/>
-      <c r="L47" s="6"/>
-    </row>
-    <row r="48" ht="18.75" customHeight="1">
-      <c r="B48" s="88" t="s">
-        <v>52</v>
-      </c>
-      <c r="F48" s="8"/>
-      <c r="G48" s="89" t="s">
-        <v>52</v>
-      </c>
-      <c r="K48" s="8"/>
-      <c r="L48" s="6"/>
-    </row>
-    <row r="49" ht="18.0" customHeight="1">
-      <c r="B49" s="7"/>
-      <c r="F49" s="8"/>
-      <c r="K49" s="8"/>
-      <c r="L49" s="6"/>
+      <c r="F49" s="50"/>
+      <c r="G49" s="95" t="s">
+        <v>42</v>
+      </c>
+      <c r="H49" s="49"/>
+      <c r="I49" s="50"/>
+      <c r="J49" s="100" t="s">
+        <v>64</v>
+      </c>
+      <c r="K49" s="49"/>
+      <c r="L49" s="7" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="50" ht="18.75" customHeight="1">
-      <c r="B50" s="7"/>
-      <c r="F50" s="8"/>
-      <c r="K50" s="8"/>
-      <c r="L50" s="6"/>
-    </row>
-    <row r="51" ht="21.0" customHeight="1">
-      <c r="B51" s="90" t="s">
-        <v>53</v>
-      </c>
-      <c r="F51" s="8"/>
-      <c r="G51" s="91" t="s">
-        <v>54</v>
-      </c>
-      <c r="K51" s="8"/>
-      <c r="L51" s="6"/>
+      <c r="B50" s="102" t="s">
+        <v>65</v>
+      </c>
+      <c r="F50" s="10"/>
+      <c r="G50" s="103" t="s">
+        <v>65</v>
+      </c>
+      <c r="K50" s="10"/>
+      <c r="L50" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" ht="18.0" customHeight="1">
+      <c r="B51" s="8"/>
+      <c r="F51" s="10"/>
+      <c r="K51" s="10"/>
+      <c r="L51" s="7" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="52" ht="18.75" customHeight="1">
-      <c r="B52" s="92" t="s">
-        <v>55</v>
-      </c>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
-      <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
-      <c r="I52" s="2"/>
-      <c r="J52" s="2"/>
-      <c r="K52" s="3"/>
-      <c r="L52" s="6"/>
-    </row>
-    <row r="53" ht="19.5" customHeight="1">
-      <c r="B53" s="93" t="s">
-        <v>56</v>
-      </c>
-      <c r="C53" s="11"/>
-      <c r="D53" s="11"/>
-      <c r="E53" s="11"/>
-      <c r="F53" s="11"/>
-      <c r="G53" s="11"/>
-      <c r="H53" s="11"/>
-      <c r="I53" s="11"/>
-      <c r="J53" s="11"/>
+      <c r="B52" s="8"/>
+      <c r="F52" s="10"/>
+      <c r="K52" s="10"/>
+      <c r="L52" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" ht="21.0" customHeight="1">
+      <c r="B53" s="104" t="s">
+        <v>66</v>
+      </c>
+      <c r="F53" s="10"/>
+      <c r="G53" s="105" t="s">
+        <v>67</v>
+      </c>
       <c r="K53" s="10"/>
-      <c r="L53" s="6"/>
-    </row>
-    <row r="54"/>
-    <row r="55"/>
+      <c r="L53" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" ht="18.75" customHeight="1">
+      <c r="B54" s="106" t="s">
+        <v>68</v>
+      </c>
+      <c r="C54" s="28"/>
+      <c r="D54" s="28"/>
+      <c r="E54" s="28"/>
+      <c r="F54" s="28"/>
+      <c r="G54" s="28"/>
+      <c r="H54" s="28"/>
+      <c r="I54" s="28"/>
+      <c r="J54" s="28"/>
+      <c r="K54" s="29"/>
+      <c r="L54" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" ht="19.5" customHeight="1">
+      <c r="B55" s="107" t="s">
+        <v>69</v>
+      </c>
+      <c r="C55" s="14"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="14"/>
+      <c r="H55" s="14"/>
+      <c r="I55" s="14"/>
+      <c r="J55" s="14"/>
+      <c r="K55" s="78"/>
+      <c r="L55" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
     <row r="56"/>
     <row r="57"/>
     <row r="58"/>
@@ -2849,40 +3249,10 @@
     <row r="999"/>
     <row r="1000"/>
     <row r="1001"/>
+    <row r="1002"/>
+    <row r="1003"/>
   </sheetData>
-  <mergeCells count="77">
-    <mergeCell ref="H41:K41"/>
-    <mergeCell ref="H42:K42"/>
-    <mergeCell ref="B36:K39"/>
-    <mergeCell ref="B40:B42"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="F40:G42"/>
-    <mergeCell ref="H40:K40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="G44:I44"/>
-    <mergeCell ref="J44:K44"/>
-    <mergeCell ref="G45:I45"/>
-    <mergeCell ref="J45:K45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="B48:F50"/>
-    <mergeCell ref="B51:F51"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="G47:I47"/>
-    <mergeCell ref="G48:K50"/>
-    <mergeCell ref="G51:K51"/>
-    <mergeCell ref="B52:K52"/>
-    <mergeCell ref="B53:K53"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="I43:K43"/>
-    <mergeCell ref="B44:B47"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="G46:I46"/>
+  <mergeCells count="83">
     <mergeCell ref="B2:D5"/>
     <mergeCell ref="E2:I5"/>
     <mergeCell ref="J2:K4"/>
@@ -2919,15 +3289,53 @@
     <mergeCell ref="B22:K25"/>
     <mergeCell ref="B26:K26"/>
     <mergeCell ref="B27:K30"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="G31:K31"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="G32:K32"/>
-    <mergeCell ref="B33:K33"/>
-    <mergeCell ref="C34:K34"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="H42:K42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="H43:K43"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F45:H45"/>
+    <mergeCell ref="I45:K45"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="G48:I48"/>
+    <mergeCell ref="J48:K48"/>
+    <mergeCell ref="G49:I49"/>
+    <mergeCell ref="J49:K49"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="B50:F52"/>
+    <mergeCell ref="G50:K52"/>
+    <mergeCell ref="B53:F53"/>
+    <mergeCell ref="G53:K53"/>
+    <mergeCell ref="B54:K54"/>
+    <mergeCell ref="B55:K55"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="E32:G34"/>
+    <mergeCell ref="I32:K34"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="H44:K44"/>
+    <mergeCell ref="B34:D34"/>
     <mergeCell ref="B35:K35"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="C36:K36"/>
+    <mergeCell ref="B37:K37"/>
+    <mergeCell ref="B38:K41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="F42:G44"/>
+    <mergeCell ref="G46:I46"/>
+    <mergeCell ref="J46:K46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="G47:I47"/>
+    <mergeCell ref="J47:K47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:F48"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.28" footer="0.0" header="0.0" left="0.17" right="0.2" top="0.15748031496062992"/>

</xml_diff>

<commit_message>
Solves bug when situation field don't is filled
</commit_message>
<xml_diff>
--- a/assets/worksheets/template-cliente.xlsx
+++ b/assets/worksheets/template-cliente.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="71">
   <si>
     <t xml:space="preserve">             </t>
   </si>
@@ -31,16 +31,19 @@
     <t>Cliente:</t>
   </si>
   <si>
-    <t xml:space="preserve">       </t>
+    <t xml:space="preserve">                                                                                     </t>
   </si>
   <si>
     <t>O.S:</t>
   </si>
   <si>
+    <t xml:space="preserve">                                                                  </t>
+  </si>
+  <si>
     <t>Local de Atendimento:</t>
   </si>
   <si>
-    <t xml:space="preserve">      </t>
+    <t xml:space="preserve">                                                                                             </t>
   </si>
   <si>
     <t xml:space="preserve">    [    ]     CORRETIVA</t>
@@ -61,6 +64,9 @@
     <t>Atendido por:</t>
   </si>
   <si>
+    <t xml:space="preserve">                                           </t>
+  </si>
+  <si>
     <t xml:space="preserve">Máquina Parada:          </t>
   </si>
   <si>
@@ -71,9 +77,6 @@
   </si>
   <si>
     <t xml:space="preserve">Garantia:          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                           </t>
   </si>
   <si>
     <t>Equipamento:</t>
@@ -394,7 +397,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="57">
+  <borders count="56">
     <border/>
     <border>
       <left style="medium">
@@ -741,17 +744,6 @@
       </bottom>
     </border>
     <border>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
@@ -812,7 +804,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="106">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -970,20 +962,13 @@
     </xf>
     <xf borderId="50" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="51" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="42" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="52" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="36" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="42" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="53" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="52" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="36" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -993,7 +978,7 @@
     <xf borderId="21" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="54" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="53" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="40" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1002,9 +987,9 @@
     <xf borderId="27" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf borderId="54" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="48" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="55" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="48" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="56" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="29" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="36" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1015,7 +1000,7 @@
     <xf borderId="40" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="55" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="54" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="48" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1024,40 +1009,43 @@
     <xf borderId="29" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf borderId="27" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="42" fillId="0" fontId="1" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="27" fillId="0" fontId="1" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="40" fillId="0" fontId="1" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="42" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="40" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="42" fillId="0" fontId="1" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="40" fillId="0" fontId="1" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="40" fillId="0" fontId="1" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="42" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="42" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="40" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="40" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="25" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="48" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="48" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="22" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="5" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="10" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1083,7 +1071,7 @@
     <xdr:ext cx="2381250" cy="0"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr descr="LOGO.jpg" id="0" name="image4.jpg"/>
+        <xdr:cNvPr descr="LOGO.jpg" id="0" name="image2.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1111,7 +1099,7 @@
     <xdr:ext cx="542925" cy="133350"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Imagem"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Imagem"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1167,7 +1155,7 @@
     <xdr:ext cx="2200275" cy="304800"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Imagem"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Imagem"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1195,7 +1183,7 @@
     <xdr:ext cx="914400" cy="304800"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Imagem"/>
+        <xdr:cNvPr id="0" name="image4.png" title="Imagem"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1223,7 +1211,7 @@
     <xdr:ext cx="914400" cy="304800"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Imagem"/>
+        <xdr:cNvPr id="0" name="image4.png" title="Imagem"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1539,7 +1527,7 @@
         <v>7</v>
       </c>
       <c r="I6" s="23" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J6" s="24"/>
       <c r="K6" s="12"/>
@@ -1549,21 +1537,21 @@
     </row>
     <row r="7" ht="12.0" customHeight="1">
       <c r="B7" s="25" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" s="26"/>
       <c r="D7" s="27" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E7" s="28"/>
       <c r="F7" s="28"/>
       <c r="G7" s="29"/>
       <c r="H7" s="30" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I7" s="29"/>
       <c r="J7" s="31" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K7" s="29"/>
       <c r="L7" s="7" t="s">
@@ -1578,11 +1566,11 @@
       <c r="F8" s="24"/>
       <c r="G8" s="12"/>
       <c r="H8" s="34" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I8" s="12"/>
       <c r="J8" s="35" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K8" s="12"/>
       <c r="L8" s="7" t="s">
@@ -1591,20 +1579,20 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="B9" s="36" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9" s="37"/>
       <c r="D9" s="38" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E9" s="39"/>
       <c r="F9" s="37"/>
       <c r="G9" s="40" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H9" s="37"/>
       <c r="I9" s="41" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="K9" s="10"/>
       <c r="L9" s="7" t="s">
@@ -1613,26 +1601,26 @@
     </row>
     <row r="10" ht="18.0" customHeight="1">
       <c r="B10" s="42" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C10" s="43"/>
       <c r="D10" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="45" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="48" t="s">
         <v>17</v>
-      </c>
-      <c r="E10" s="45" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="46" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="44" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="47" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" s="48" t="s">
-        <v>20</v>
       </c>
       <c r="J10" s="49"/>
       <c r="K10" s="50"/>
@@ -1642,10 +1630,10 @@
     </row>
     <row r="11" ht="16.5" customHeight="1">
       <c r="B11" s="51" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11" s="52" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D11" s="21"/>
       <c r="E11" s="21"/>
@@ -1661,10 +1649,10 @@
     </row>
     <row r="12" ht="16.5" customHeight="1">
       <c r="B12" s="54" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C12" s="55" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D12" s="39"/>
       <c r="E12" s="39"/>
@@ -1680,7 +1668,7 @@
     </row>
     <row r="13" ht="12.0" customHeight="1">
       <c r="B13" s="57" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C13" s="49"/>
       <c r="D13" s="49"/>
@@ -1697,23 +1685,23 @@
     </row>
     <row r="14" ht="25.5" customHeight="1">
       <c r="B14" s="58" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="59" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="60" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H14" s="10"/>
       <c r="I14" s="60" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J14" s="10"/>
       <c r="K14" s="61" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L14" s="7" t="s">
         <v>3</v>
@@ -1721,21 +1709,21 @@
     </row>
     <row r="15" ht="21.0" customHeight="1">
       <c r="B15" s="62" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C15" s="50"/>
       <c r="D15" s="63" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E15" s="50"/>
       <c r="F15" s="64" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G15" s="49"/>
       <c r="H15" s="49"/>
       <c r="I15" s="50"/>
       <c r="J15" s="65" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K15" s="50"/>
       <c r="L15" s="7" t="s">
@@ -1744,7 +1732,7 @@
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="B16" s="66" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C16" s="24"/>
       <c r="D16" s="24"/>
@@ -1761,7 +1749,7 @@
     </row>
     <row r="17" ht="18.75" customHeight="1">
       <c r="B17" s="67" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K17" s="10"/>
       <c r="L17" s="7" t="s">
@@ -1791,7 +1779,7 @@
     </row>
     <row r="21" ht="16.5" customHeight="1">
       <c r="B21" s="68" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C21" s="49"/>
       <c r="D21" s="49"/>
@@ -1808,7 +1796,7 @@
     </row>
     <row r="22" ht="18.75" customHeight="1">
       <c r="B22" s="67" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K22" s="10"/>
       <c r="L22" s="7" t="s">
@@ -1838,7 +1826,7 @@
     </row>
     <row r="26" ht="13.5" customHeight="1">
       <c r="B26" s="68" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C26" s="49"/>
       <c r="D26" s="49"/>
@@ -1855,7 +1843,7 @@
     </row>
     <row r="27" ht="18.75" customHeight="1">
       <c r="B27" s="67" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K27" s="10"/>
       <c r="L27" s="7" t="s">
@@ -1885,43 +1873,43 @@
     </row>
     <row r="31" ht="18.75" customHeight="1">
       <c r="B31" s="69" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C31" s="49"/>
       <c r="D31" s="49"/>
       <c r="E31" s="70" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F31" s="71"/>
-      <c r="G31" s="72"/>
-      <c r="H31" s="73" t="s">
-        <v>40</v>
+      <c r="G31" s="71"/>
+      <c r="H31" s="69" t="s">
+        <v>41</v>
       </c>
       <c r="I31" s="70" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J31" s="71"/>
-      <c r="K31" s="74"/>
+      <c r="K31" s="72"/>
       <c r="L31" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="32" ht="18.75" customHeight="1">
       <c r="B32" s="69" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C32" s="49"/>
       <c r="D32" s="49"/>
-      <c r="E32" s="75" t="s">
-        <v>42</v>
+      <c r="E32" s="73" t="s">
+        <v>43</v>
       </c>
       <c r="F32" s="2"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="73" t="s">
-        <v>40</v>
-      </c>
-      <c r="I32" s="75" t="s">
-        <v>12</v>
+      <c r="G32" s="2"/>
+      <c r="H32" s="69" t="s">
+        <v>41</v>
+      </c>
+      <c r="I32" s="73" t="s">
+        <v>13</v>
       </c>
       <c r="J32" s="2"/>
       <c r="K32" s="6"/>
@@ -1931,14 +1919,13 @@
     </row>
     <row r="33" ht="18.75" customHeight="1">
       <c r="B33" s="69" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C33" s="49"/>
       <c r="D33" s="49"/>
       <c r="E33" s="8"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="73" t="s">
-        <v>40</v>
+      <c r="H33" s="69" t="s">
+        <v>41</v>
       </c>
       <c r="I33" s="8"/>
       <c r="K33" s="10"/>
@@ -1947,27 +1934,27 @@
       </c>
     </row>
     <row r="34" ht="18.75" customHeight="1">
-      <c r="B34" s="76" t="s">
-        <v>20</v>
+      <c r="B34" s="74" t="s">
+        <v>17</v>
       </c>
       <c r="C34" s="49"/>
       <c r="D34" s="49"/>
       <c r="E34" s="13"/>
       <c r="F34" s="14"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="77" t="s">
-        <v>40</v>
+      <c r="G34" s="14"/>
+      <c r="H34" s="74" t="s">
+        <v>41</v>
       </c>
       <c r="I34" s="13"/>
       <c r="J34" s="14"/>
-      <c r="K34" s="78"/>
+      <c r="K34" s="75"/>
       <c r="L34" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="35" ht="18.75" customHeight="1">
-      <c r="B35" s="79" t="s">
-        <v>20</v>
+      <c r="B35" s="76" t="s">
+        <v>17</v>
       </c>
       <c r="C35" s="49"/>
       <c r="D35" s="49"/>
@@ -1983,11 +1970,11 @@
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="B36" s="80" t="s">
-        <v>43</v>
-      </c>
-      <c r="C36" s="81" t="s">
+      <c r="B36" s="77" t="s">
         <v>44</v>
+      </c>
+      <c r="C36" s="78" t="s">
+        <v>45</v>
       </c>
       <c r="D36" s="24"/>
       <c r="E36" s="24"/>
@@ -2003,7 +1990,7 @@
     </row>
     <row r="37" ht="18.0" customHeight="1">
       <c r="B37" s="66" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C37" s="24"/>
       <c r="D37" s="24"/>
@@ -2020,7 +2007,7 @@
     </row>
     <row r="38" ht="18.75" customHeight="1">
       <c r="B38" s="67" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="K38" s="10"/>
       <c r="L38" s="7" t="s">
@@ -2049,20 +2036,20 @@
       </c>
     </row>
     <row r="42" ht="15.0" customHeight="1">
-      <c r="B42" s="82" t="s">
-        <v>46</v>
-      </c>
-      <c r="C42" s="83" t="s">
+      <c r="B42" s="79" t="s">
         <v>47</v>
+      </c>
+      <c r="C42" s="80" t="s">
+        <v>48</v>
       </c>
       <c r="D42" s="49"/>
       <c r="E42" s="50"/>
-      <c r="F42" s="84" t="s">
+      <c r="F42" s="81" t="s">
+        <v>49</v>
+      </c>
+      <c r="G42" s="29"/>
+      <c r="H42" s="80" t="s">
         <v>48</v>
-      </c>
-      <c r="G42" s="29"/>
-      <c r="H42" s="83" t="s">
-        <v>47</v>
       </c>
       <c r="I42" s="49"/>
       <c r="J42" s="49"/>
@@ -2072,16 +2059,16 @@
       </c>
     </row>
     <row r="43" ht="15.0" customHeight="1">
-      <c r="B43" s="85"/>
-      <c r="C43" s="83" t="s">
-        <v>49</v>
+      <c r="B43" s="82"/>
+      <c r="C43" s="80" t="s">
+        <v>50</v>
       </c>
       <c r="D43" s="49"/>
       <c r="E43" s="50"/>
-      <c r="F43" s="86"/>
+      <c r="F43" s="83"/>
       <c r="G43" s="10"/>
-      <c r="H43" s="83" t="s">
-        <v>49</v>
+      <c r="H43" s="80" t="s">
+        <v>50</v>
       </c>
       <c r="I43" s="49"/>
       <c r="J43" s="49"/>
@@ -2091,16 +2078,16 @@
       </c>
     </row>
     <row r="44" ht="15.0" customHeight="1">
-      <c r="B44" s="87"/>
-      <c r="C44" s="83" t="s">
-        <v>50</v>
+      <c r="B44" s="84"/>
+      <c r="C44" s="80" t="s">
+        <v>51</v>
       </c>
       <c r="D44" s="49"/>
       <c r="E44" s="50"/>
-      <c r="F44" s="88"/>
+      <c r="F44" s="85"/>
       <c r="G44" s="12"/>
-      <c r="H44" s="83" t="s">
-        <v>50</v>
+      <c r="H44" s="80" t="s">
+        <v>51</v>
       </c>
       <c r="I44" s="49"/>
       <c r="J44" s="49"/>
@@ -2110,21 +2097,21 @@
       </c>
     </row>
     <row r="45" ht="18.0" customHeight="1">
-      <c r="B45" s="89" t="s">
-        <v>51</v>
+      <c r="B45" s="86" t="s">
+        <v>52</v>
       </c>
       <c r="C45" s="43"/>
-      <c r="D45" s="90" t="s">
-        <v>31</v>
+      <c r="D45" s="87" t="s">
+        <v>32</v>
       </c>
       <c r="E45" s="43"/>
-      <c r="F45" s="91" t="s">
-        <v>52</v>
+      <c r="F45" s="88" t="s">
+        <v>53</v>
       </c>
       <c r="G45" s="49"/>
       <c r="H45" s="50"/>
-      <c r="I45" s="91" t="s">
-        <v>53</v>
+      <c r="I45" s="88" t="s">
+        <v>54</v>
       </c>
       <c r="J45" s="49"/>
       <c r="K45" s="50"/>
@@ -2133,24 +2120,24 @@
       </c>
     </row>
     <row r="46">
-      <c r="B46" s="92" t="s">
-        <v>54</v>
-      </c>
-      <c r="C46" s="93" t="s">
+      <c r="B46" s="89" t="s">
         <v>55</v>
       </c>
+      <c r="C46" s="90" t="s">
+        <v>56</v>
+      </c>
       <c r="D46" s="10"/>
-      <c r="E46" s="93" t="s">
-        <v>56</v>
+      <c r="E46" s="90" t="s">
+        <v>57</v>
       </c>
       <c r="F46" s="10"/>
-      <c r="G46" s="94" t="s">
-        <v>57</v>
+      <c r="G46" s="91" t="s">
+        <v>58</v>
       </c>
       <c r="H46" s="24"/>
       <c r="I46" s="12"/>
-      <c r="J46" s="94" t="s">
-        <v>58</v>
+      <c r="J46" s="91" t="s">
+        <v>59</v>
       </c>
       <c r="K46" s="12"/>
       <c r="L46" s="7" t="s">
@@ -2158,21 +2145,21 @@
       </c>
     </row>
     <row r="47">
-      <c r="B47" s="85"/>
-      <c r="C47" s="95" t="s">
-        <v>59</v>
-      </c>
-      <c r="D47" s="50"/>
-      <c r="E47" s="96">
+      <c r="B47" s="82"/>
+      <c r="C47" s="92" t="s">
+        <v>60</v>
+      </c>
+      <c r="D47" s="29"/>
+      <c r="E47" s="93">
         <v>0.0</v>
       </c>
       <c r="F47" s="50"/>
-      <c r="G47" s="97">
+      <c r="G47" s="94">
         <v>0.0</v>
       </c>
-      <c r="H47" s="49"/>
-      <c r="I47" s="50"/>
-      <c r="J47" s="98">
+      <c r="H47" s="28"/>
+      <c r="I47" s="29"/>
+      <c r="J47" s="95">
         <f>G47-E47</f>
         <v>0</v>
       </c>
@@ -2182,22 +2169,22 @@
       </c>
     </row>
     <row r="48">
-      <c r="B48" s="85"/>
-      <c r="C48" s="95" t="s">
-        <v>60</v>
-      </c>
-      <c r="D48" s="50"/>
-      <c r="E48" s="99" t="s">
+      <c r="B48" s="82"/>
+      <c r="C48" s="96" t="s">
         <v>61</v>
       </c>
+      <c r="D48" s="49"/>
+      <c r="E48" s="97" t="s">
+        <v>62</v>
+      </c>
       <c r="F48" s="50"/>
-      <c r="G48" s="95" t="s">
-        <v>62</v>
+      <c r="G48" s="97" t="s">
+        <v>63</v>
       </c>
       <c r="H48" s="49"/>
-      <c r="I48" s="50"/>
-      <c r="J48" s="100" t="s">
-        <v>63</v>
+      <c r="I48" s="49"/>
+      <c r="J48" s="98" t="s">
+        <v>64</v>
       </c>
       <c r="K48" s="50"/>
       <c r="L48" s="7" t="s">
@@ -2205,22 +2192,22 @@
       </c>
     </row>
     <row r="49">
-      <c r="B49" s="87"/>
-      <c r="C49" s="101" t="s">
-        <v>42</v>
-      </c>
-      <c r="D49" s="50"/>
-      <c r="E49" s="99" t="s">
-        <v>42</v>
-      </c>
-      <c r="F49" s="50"/>
-      <c r="G49" s="95" t="s">
-        <v>42</v>
+      <c r="B49" s="84"/>
+      <c r="C49" s="99" t="s">
+        <v>43</v>
+      </c>
+      <c r="D49" s="28"/>
+      <c r="E49" s="92" t="s">
+        <v>43</v>
+      </c>
+      <c r="F49" s="29"/>
+      <c r="G49" s="97" t="s">
+        <v>43</v>
       </c>
       <c r="H49" s="49"/>
-      <c r="I49" s="50"/>
-      <c r="J49" s="100" t="s">
-        <v>64</v>
+      <c r="I49" s="49"/>
+      <c r="J49" s="98" t="s">
+        <v>65</v>
       </c>
       <c r="K49" s="49"/>
       <c r="L49" s="7" t="s">
@@ -2228,12 +2215,11 @@
       </c>
     </row>
     <row r="50" ht="18.75" customHeight="1">
-      <c r="B50" s="102" t="s">
-        <v>65</v>
-      </c>
-      <c r="F50" s="10"/>
-      <c r="G50" s="103" t="s">
-        <v>65</v>
+      <c r="B50" s="100" t="s">
+        <v>66</v>
+      </c>
+      <c r="G50" s="101" t="s">
+        <v>66</v>
       </c>
       <c r="K50" s="10"/>
       <c r="L50" s="7" t="s">
@@ -2242,7 +2228,7 @@
     </row>
     <row r="51" ht="18.0" customHeight="1">
       <c r="B51" s="8"/>
-      <c r="F51" s="10"/>
+      <c r="G51" s="83"/>
       <c r="K51" s="10"/>
       <c r="L51" s="7" t="s">
         <v>3</v>
@@ -2250,19 +2236,18 @@
     </row>
     <row r="52" ht="18.75" customHeight="1">
       <c r="B52" s="8"/>
-      <c r="F52" s="10"/>
+      <c r="G52" s="83"/>
       <c r="K52" s="10"/>
       <c r="L52" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="53" ht="21.0" customHeight="1">
-      <c r="B53" s="104" t="s">
-        <v>66</v>
-      </c>
-      <c r="F53" s="10"/>
-      <c r="G53" s="105" t="s">
+      <c r="B53" s="102" t="s">
         <v>67</v>
+      </c>
+      <c r="G53" s="103" t="s">
+        <v>68</v>
       </c>
       <c r="K53" s="10"/>
       <c r="L53" s="7" t="s">
@@ -2270,25 +2255,17 @@
       </c>
     </row>
     <row r="54" ht="18.75" customHeight="1">
-      <c r="B54" s="106" t="s">
-        <v>68</v>
-      </c>
-      <c r="C54" s="28"/>
-      <c r="D54" s="28"/>
-      <c r="E54" s="28"/>
-      <c r="F54" s="28"/>
-      <c r="G54" s="28"/>
-      <c r="H54" s="28"/>
-      <c r="I54" s="28"/>
-      <c r="J54" s="28"/>
-      <c r="K54" s="29"/>
+      <c r="B54" s="104" t="s">
+        <v>69</v>
+      </c>
+      <c r="K54" s="10"/>
       <c r="L54" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="55" ht="19.5" customHeight="1">
-      <c r="B55" s="107" t="s">
-        <v>69</v>
+      <c r="B55" s="105" t="s">
+        <v>70</v>
       </c>
       <c r="C55" s="14"/>
       <c r="D55" s="14"/>
@@ -2298,7 +2275,7 @@
       <c r="H55" s="14"/>
       <c r="I55" s="14"/>
       <c r="J55" s="14"/>
-      <c r="K55" s="78"/>
+      <c r="K55" s="75"/>
       <c r="L55" s="7" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Update some silly things
</commit_message>
<xml_diff>
--- a/assets/worksheets/template-cliente.xlsx
+++ b/assets/worksheets/template-cliente.xlsx
@@ -208,7 +208,7 @@
     <t>SITUAÇÃO:</t>
   </si>
   <si>
-    <t>[   ] LIBERADO                     [   ] LIBERADO COM RESTRIÇÕES                [   ] NÃO LIBERADO                [   ] FALTA PEÇAS</t>
+    <t>[   ] LIBERADO     [   ] LIBERADO COM RESTRIÇÕES    [   ] NÃO LIBERADO    [   ] FALTA PEÇAS</t>
   </si>
   <si>
     <t>PENDÊNCIAS:</t>
@@ -1071,7 +1071,7 @@
     <xdr:ext cx="2381250" cy="0"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr descr="LOGO.jpg" id="0" name="image2.jpg"/>
+        <xdr:cNvPr descr="LOGO.jpg" id="0" name="image5.jpg"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1099,7 +1099,7 @@
     <xdr:ext cx="542925" cy="133350"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Imagem"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Imagem"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1127,7 +1127,7 @@
     <xdr:ext cx="571500" cy="104775"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.png" title="Imagem"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Imagem"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1155,7 +1155,7 @@
     <xdr:ext cx="2200275" cy="304800"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Imagem"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Imagem"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3270,25 +3270,25 @@
     <mergeCell ref="H42:K42"/>
     <mergeCell ref="C43:E43"/>
     <mergeCell ref="H43:K43"/>
-    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="G48:I48"/>
+    <mergeCell ref="J48:K48"/>
     <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="B50:F52"/>
+    <mergeCell ref="B53:F53"/>
+    <mergeCell ref="G49:I49"/>
+    <mergeCell ref="J49:K49"/>
+    <mergeCell ref="G50:K52"/>
+    <mergeCell ref="G53:K53"/>
+    <mergeCell ref="B54:K54"/>
+    <mergeCell ref="B55:K55"/>
     <mergeCell ref="B45:C45"/>
     <mergeCell ref="D45:E45"/>
     <mergeCell ref="F45:H45"/>
     <mergeCell ref="I45:K45"/>
     <mergeCell ref="B46:B49"/>
+    <mergeCell ref="C46:D46"/>
     <mergeCell ref="E46:F46"/>
-    <mergeCell ref="G48:I48"/>
-    <mergeCell ref="J48:K48"/>
-    <mergeCell ref="G49:I49"/>
-    <mergeCell ref="J49:K49"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="B50:F52"/>
-    <mergeCell ref="G50:K52"/>
-    <mergeCell ref="B53:F53"/>
-    <mergeCell ref="G53:K53"/>
-    <mergeCell ref="B54:K54"/>
-    <mergeCell ref="B55:K55"/>
     <mergeCell ref="B31:D31"/>
     <mergeCell ref="E31:G31"/>
     <mergeCell ref="I31:K31"/>
@@ -3315,7 +3315,7 @@
     <mergeCell ref="E48:F48"/>
   </mergeCells>
   <printOptions/>
-  <pageMargins bottom="0.28" footer="0.0" header="0.0" left="0.17" right="0.2" top="0.15748031496062992"/>
+  <pageMargins bottom="0.28" footer="0.0" header="0.0" left="0.2578740157480315" right="0.2" top="0.15748031496062992"/>
   <pageSetup paperSize="9" scale="84" orientation="portrait"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>